<commit_message>
Added command line options to control compatibility hacks.
Enabled overrides for the date and the time, which is useful for
bypassing "prime time" hours when the cave is closed, proving you're
a wizard, avoiding Y2K bugs, and getting a reproducible seed for the
random number generator.

Added an option to disable the Y2K hack (which is enabled by default).

Extended the Wizard spreadsheet to show the magic word calculation if
you override the clock to 1977-01-01 00:00.

Added options to get a summary of the options.
</commit_message>
<xml_diff>
--- a/tools/wizard.xlsx
+++ b/tools/wizard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\aid\experimental\fortran\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\fortran-adventure\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F4E2D2-3888-4905-8B93-C3B03D1E2CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0735A-D652-4D8E-AF43-3E76FC6A3714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="17914" xr2:uid="{EA4EB66F-FA79-46BF-BDB7-6DBFA30FB5E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Y</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Minutes</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Very first turn</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Copy the challenge word into column B below.</t>
   </si>
   <si>
-    <t>Respond with the response in column I below.</t>
-  </si>
-  <si>
     <t>The correct response changes every 10 minutes.</t>
   </si>
   <si>
@@ -99,10 +93,16 @@
     <t>MAGNUM</t>
   </si>
   <si>
-    <t>RISMF</t>
-  </si>
-  <si>
     <t>|delta|</t>
+  </si>
+  <si>
+    <t>Respond with the response in column H below.</t>
+  </si>
+  <si>
+    <t>FSMDA</t>
+  </si>
+  <si>
+    <t>Run Adventure with -d1-JAN-77 -t0:00 to lock the date and time and simplify the calculation.</t>
   </si>
 </sst>
 </file>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82230EC-4216-4B92-A2D9-410B51CF2B56}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -500,34 +500,34 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
@@ -540,17 +540,17 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -560,8 +560,8 @@
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
-        <v>23</v>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>9</v>
@@ -573,7 +573,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="5">
         <f ca="1">NOW()</f>
-        <v>45797.576716898147</v>
+        <v>45804.656044444448</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
@@ -583,11 +583,11 @@
       </c>
       <c r="F14" s="3">
         <f ca="1">60*HOUR(A14)+MINUTE(A14)</f>
-        <v>830</v>
+        <v>944</v>
       </c>
       <c r="H14" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(H16:H20)</f>
-        <v>JPJIM</v>
+        <v>NKOEF</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -595,15 +595,15 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -613,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
@@ -622,15 +622,15 @@
       </c>
       <c r="B16" s="1" t="str">
         <f>UPPER(MID(B14, A16, 1))</f>
-        <v>R</v>
+        <v>F</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C20" si="0">CODE(UPPER(B16)) - CODE("A") + 1</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <f>ABS(C16-C17)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E16">
         <f>E14</f>
@@ -638,15 +638,15 @@
       </c>
       <c r="F16">
         <f ca="1">40*FLOOR(F14/60, 1)+10*FLOOR(F14/10,1)</f>
-        <v>1350</v>
+        <v>1540</v>
       </c>
       <c r="G16">
         <f ca="1">MOD(D16*MOD(E16, 10)+MOD(F16, 10), 26)+1</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H16" s="4" t="str">
         <f ca="1">CHAR(64+G16)</f>
-        <v>J</v>
+        <v>N</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
@@ -655,15 +655,15 @@
       </c>
       <c r="B17" s="1" t="str">
         <f>UPPER(MID(B14, A17, 1))</f>
-        <v>I</v>
+        <v>S</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <f>ABS(C17-C18)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <f>FLOOR(E16/10, 1)</f>
@@ -671,15 +671,15 @@
       </c>
       <c r="F17">
         <f ca="1">FLOOR(F16/10, 1)</f>
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="G17">
         <f ca="1">MOD(D17*MOD(E17, 10)+MOD(F17, 10), 26)+1</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H17" s="4" t="str">
         <f t="shared" ref="H17:H20" ca="1" si="1">CHAR(64+G17)</f>
-        <v>P</v>
+        <v>K</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
@@ -688,15 +688,15 @@
       </c>
       <c r="B18" s="1" t="str">
         <f>UPPER(MID(B14, A18, 1))</f>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <f>ABS(C18-C19)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <f>FLOOR(E17/10, 1)</f>
@@ -704,15 +704,15 @@
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F20" ca="1" si="2">FLOOR(F17/10, 1)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G18">
         <f ca="1">MOD(D18*MOD(E18, 10)+MOD(F18, 10), 26)+1</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H18" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>J</v>
+        <v>O</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
@@ -721,15 +721,15 @@
       </c>
       <c r="B19" s="1" t="str">
         <f>UPPER(MID(B14, A19, 1))</f>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f>ABS(C19-C20)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <f>FLOOR(E18/10, 1)</f>
@@ -741,11 +741,11 @@
       </c>
       <c r="G19">
         <f ca="1">MOD(D19*MOD(E19, 10)+MOD(F19, 10), 26)+1</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H19" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>I</v>
+        <v>E</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
@@ -754,15 +754,15 @@
       </c>
       <c r="B20" s="1" t="str">
         <f>UPPER(MID(B14, A20, 1))</f>
-        <v>F</v>
+        <v>A</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <f>ABS(C20-C16)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>FLOOR(E19/10, 1)</f>
@@ -774,21 +774,243 @@
       </c>
       <c r="G20">
         <f ca="1">MOD(D20*MOD(E20, 10)+MOD(F20, 10), 26)+1</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H20" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <v>28126</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>11111</v>
+      </c>
+      <c r="F24" s="3">
+        <f>60*HOUR(A24)+MINUTE(A24)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f>_xlfn.CONCAT(H26:H30)</f>
+        <v>NGJDF</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>UPPER(MID(B24, A26, 1))</f>
+        <v>F</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C30" si="3">CODE(UPPER(B26)) - CODE("A") + 1</f>
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <f>ABS(C26-C27)</f>
+        <v>13</v>
+      </c>
+      <c r="E26">
+        <f>E24</f>
+        <v>11111</v>
+      </c>
+      <c r="F26">
+        <f>40*FLOOR(F24/60, 1)+10*FLOOR(F24/10,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>MOD(D26*MOD(E26, 10)+MOD(F26, 10), 26)+1</f>
+        <v>14</v>
+      </c>
+      <c r="H26" s="4" t="str">
+        <f>CHAR(64+G26)</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f>UPPER(MID(B24, A27, 1))</f>
+        <v>S</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <f>ABS(C27-C28)</f>
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <f>FLOOR(E26/10, 1)</f>
+        <v>1111</v>
+      </c>
+      <c r="F27">
+        <f>FLOOR(F26/10, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>MOD(D27*MOD(E27, 10)+MOD(F27, 10), 26)+1</f>
+        <v>7</v>
+      </c>
+      <c r="H27" s="4" t="str">
+        <f t="shared" ref="H27:H30" si="4">CHAR(64+G27)</f>
+        <v>G</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f>UPPER(MID(B24, A28, 1))</f>
         <v>M</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <f>ABS(C28-C29)</f>
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <f>FLOOR(E27/10, 1)</f>
+        <v>111</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F30" si="5">FLOOR(F27/10, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>MOD(D28*MOD(E28, 10)+MOD(F28, 10), 26)+1</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B25" t="s">
-        <v>10</v>
+      <c r="H28" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>J</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f>UPPER(MID(B24, A29, 1))</f>
+        <v>D</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <f>ABS(C29-C30)</f>
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <f>FLOOR(E28/10, 1)</f>
+        <v>11</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f>MOD(D29*MOD(E29, 10)+MOD(F29, 10), 26)+1</f>
+        <v>4</v>
+      </c>
+      <c r="H29" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f>UPPER(MID(B24, A30, 1))</f>
+        <v>A</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f>ABS(C30-C26)</f>
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <f>FLOOR(E29/10, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>MOD(D30*MOD(E30, 10)+MOD(F30, 10), 26)+1</f>
+        <v>6</v>
+      </c>
+      <c r="H30" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved (somewhat) the core image saving and loading.
* File names are sanitized and a default file extension can be applied.
* An atexit handler ensures the user gets can save a core image.
  Unfortunately, we don't really want to offer that on every exit.
* This enabled removal of the Big Ol' Hack.
* Used the wizard mode spreadsheet with a different fixed time in order
  to continue my first-ever saved game!
</commit_message>
<xml_diff>
--- a/tools/wizard.xlsx
+++ b/tools/wizard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\fortran-adventure\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0735A-D652-4D8E-AF43-3E76FC6A3714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C5DED1-D664-41B2-B36C-5E2C787CC3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="17914" xr2:uid="{EA4EB66F-FA79-46BF-BDB7-6DBFA30FB5E4}"/>
+    <workbookView xWindow="34" yWindow="1277" windowWidth="16423" windowHeight="15712" xr2:uid="{EA4EB66F-FA79-46BF-BDB7-6DBFA30FB5E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>Y</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Run Adventure with -d1-JAN-77 -t0:00 to lock the date and time and simplify the calculation.</t>
+  </si>
+  <si>
+    <t>Run Adventure with -d1-JAN-77 -t0:31 to lock the date and time and simplify the calculation.</t>
+  </si>
+  <si>
+    <t>WODSE</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82230EC-4216-4B92-A2D9-410B51CF2B56}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -573,7 +579,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="5">
         <f ca="1">NOW()</f>
-        <v>45804.656044444448</v>
+        <v>46040.462223495371</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
@@ -583,11 +589,11 @@
       </c>
       <c r="F14" s="3">
         <f ca="1">60*HOUR(A14)+MINUTE(A14)</f>
-        <v>944</v>
+        <v>665</v>
       </c>
       <c r="H14" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(H16:H20)</f>
-        <v>NKOEF</v>
+        <v>NGKEF</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -638,7 +644,7 @@
       </c>
       <c r="F16">
         <f ca="1">40*FLOOR(F14/60, 1)+10*FLOOR(F14/10,1)</f>
-        <v>1540</v>
+        <v>1100</v>
       </c>
       <c r="G16">
         <f ca="1">MOD(D16*MOD(E16, 10)+MOD(F16, 10), 26)+1</f>
@@ -671,15 +677,15 @@
       </c>
       <c r="F17">
         <f ca="1">FLOOR(F16/10, 1)</f>
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="G17">
         <f ca="1">MOD(D17*MOD(E17, 10)+MOD(F17, 10), 26)+1</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H17" s="4" t="str">
         <f t="shared" ref="H17:H20" ca="1" si="1">CHAR(64+G17)</f>
-        <v>K</v>
+        <v>G</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
@@ -704,15 +710,15 @@
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F20" ca="1" si="2">FLOOR(F17/10, 1)</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G18">
         <f ca="1">MOD(D18*MOD(E18, 10)+MOD(F18, 10), 26)+1</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H18" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>O</v>
+        <v>K</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
@@ -1011,6 +1017,238 @@
       <c r="H30" s="4" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" s="5">
+        <v>28126.021527777779</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34">
+        <v>11111</v>
+      </c>
+      <c r="F34" s="3">
+        <f>60*HOUR(A34)+MINUTE(A34)</f>
+        <v>31</v>
+      </c>
+      <c r="H34" s="4" t="str">
+        <f>_xlfn.CONCAT(H36:H40)</f>
+        <v>IOPOS</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f>UPPER(MID(B34, A36, 1))</f>
+        <v>W</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:C40" si="6">CODE(UPPER(B36)) - CODE("A") + 1</f>
+        <v>23</v>
+      </c>
+      <c r="D36">
+        <f>ABS(C36-C37)</f>
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <f>E34</f>
+        <v>11111</v>
+      </c>
+      <c r="F36">
+        <f>40*FLOOR(F34/60, 1)+10*FLOOR(F34/10,1)</f>
+        <v>30</v>
+      </c>
+      <c r="G36">
+        <f>MOD(D36*MOD(E36, 10)+MOD(F36, 10), 26)+1</f>
+        <v>9</v>
+      </c>
+      <c r="H36" s="4" t="str">
+        <f>CHAR(64+G36)</f>
+        <v>I</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f>UPPER(MID(B34, A37, 1))</f>
+        <v>O</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <f>ABS(C37-C38)</f>
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <f>FLOOR(E36/10, 1)</f>
+        <v>1111</v>
+      </c>
+      <c r="F37">
+        <f>FLOOR(F36/10, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <f>MOD(D37*MOD(E37, 10)+MOD(F37, 10), 26)+1</f>
+        <v>15</v>
+      </c>
+      <c r="H37" s="4" t="str">
+        <f t="shared" ref="H37:H40" si="7">CHAR(64+G37)</f>
+        <v>O</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f>UPPER(MID(B34, A38, 1))</f>
+        <v>D</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <f>ABS(C38-C39)</f>
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <f>FLOOR(E37/10, 1)</f>
+        <v>111</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ref="F38:F40" si="8">FLOOR(F37/10, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f>MOD(D38*MOD(E38, 10)+MOD(F38, 10), 26)+1</f>
+        <v>16</v>
+      </c>
+      <c r="H38" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f>UPPER(MID(B34, A39, 1))</f>
+        <v>S</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="D39">
+        <f>ABS(C39-C40)</f>
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <f>FLOOR(E38/10, 1)</f>
+        <v>11</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f>MOD(D39*MOD(E39, 10)+MOD(F39, 10), 26)+1</f>
+        <v>15</v>
+      </c>
+      <c r="H39" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>O</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>UPPER(MID(B34, A40, 1))</f>
+        <v>E</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <f>ABS(C40-C36)</f>
+        <v>18</v>
+      </c>
+      <c r="E40">
+        <f>FLOOR(E39/10, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f>MOD(D40*MOD(E40, 10)+MOD(F40, 10), 26)+1</f>
+        <v>19</v>
+      </c>
+      <c r="H40" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
       </c>
     </row>
   </sheetData>

</xml_diff>